<commit_message>
Modifying the simulator to be fast for vriksha purposes
</commit_message>
<xml_diff>
--- a/VrikshaSim/Results/Description.xlsx
+++ b/VrikshaSim/Results/Description.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19380"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>First results comparing TCP/EDF/Vriksha - Saw that while network time parts of Vriksha look bad, it seems to do well for the response times but not too well.</t>
   </si>
@@ -49,6 +49,129 @@
   </si>
   <si>
     <t>Running Ion's experiments about the variation of meeting end to end deadlines for exponential and normal distributions.</t>
+  </si>
+  <si>
+    <t>12/14/12</t>
+  </si>
+  <si>
+    <t>If I make all the requests to be of same time, but make the tasks along a particular request variable, then I see virtually no improvement with Vriksha at low loads</t>
+  </si>
+  <si>
+    <t>12/15/12</t>
+  </si>
+  <si>
+    <t>Keep a steady timeout, and vary request specific computation times and see the utility values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SimulationsNormalDiffRequestsSameTimeout.txt </t>
+  </si>
+  <si>
+    <t>MLA and Worker time = 100ms, 50ms, stdev across requests 30%, within request 20%, deadline values 200, 220, 240</t>
+  </si>
+  <si>
+    <t>For different values of worker and mla wait times, find the optimal waiting time value -- stored in optimal.txt. Changed stdev to be 40% across requests, within request is still the same</t>
+  </si>
+  <si>
+    <t>Optimal.txt</t>
+  </si>
+  <si>
+    <t>StaticTimeOuts.txt</t>
+  </si>
+  <si>
+    <t>Same normal distribution, but with 180ms deadline at the HLA. The optimal values used were from Optimal.txt (that used 200ms as deadline so there is an inconsistency).</t>
+  </si>
+  <si>
+    <t>OptimalWrtStdev..</t>
+  </si>
+  <si>
+    <t>For Normal Distribution, I take equal stage times (100 ms each), set the deadline to 280ms, and vary stdev (same for both stages) to observe the change in utility values</t>
+  </si>
+  <si>
+    <t>Similarly for exponential distribution also (change the maximum value).</t>
+  </si>
+  <si>
+    <t>See Jeff Dean's numbers and seeing how to fit distributions (Exponential maybe)</t>
+  </si>
+  <si>
+    <t>Used R --&gt; Installed rriskDistributions package. Install modules (R CMD INSTALL) and run the function in the documentation</t>
+  </si>
+  <si>
+    <t>Came out to be log-normal distribution with parameters:: mean = 2.94, sigma=0.54.</t>
+  </si>
+  <si>
+    <t>OptimalLogNormal.py</t>
+  </si>
+  <si>
+    <t>For the Log Normal parameters, mean = 2.94, sigma = 0.55 from Jeff Dean's presentation</t>
+  </si>
+  <si>
+    <t>Median = 18, 99% = 67, 99.9 = 100; Varied the value of deadline from 50 to 150ms and saw how utility varies with different wait times</t>
+  </si>
+  <si>
+    <t>Investigate whether the analytical model holds for the LogNormal Distribution</t>
+  </si>
+  <si>
+    <t>CheckDeltaUAnalysis.py - For normal distributions, Check from Python if the Delta utility analysis holds.</t>
+  </si>
+  <si>
+    <t>CheckDeltaUAnalysis.py - In this case for log-normal distribution.</t>
+  </si>
+  <si>
+    <t>Contrast with respect to fanout, how it changes for different fanouts -- In above the deadline of 90 seems to go down so I picked that</t>
+  </si>
+  <si>
+    <t>Change the parameters of the second stage, and then simulate varying deadlines again. I made the second stage so that it's mean is 38, same stdev but mean = 3.5 (Still LogNormal)</t>
+  </si>
+  <si>
+    <t>DeltaUAnalysisForFanout.py</t>
+  </si>
+  <si>
+    <t>OptimalLogNormalDiffStageTimes.py</t>
+  </si>
+  <si>
+    <t>Achieved both using simulation and analysis.</t>
+  </si>
+  <si>
+    <t>Moving towards the goal to finish plot requested by Sylvia.</t>
+  </si>
+  <si>
+    <t>X2 ~ 3.4 mean, stdev of 0.4 and then task times are Log-normal with stdev of 0.55</t>
+  </si>
+  <si>
+    <t>X1 ~ 2.9 mean, stdev of 0.35 and then task times are Log-normal with sigma 0.55</t>
+  </si>
+  <si>
+    <t>Meeting with Ion</t>
+  </si>
+  <si>
+    <t>Things to do: Pick equal distributions for the both of the stages.</t>
+  </si>
+  <si>
+    <t>How about you send half of it to check with the aggregator.</t>
+  </si>
+  <si>
+    <t>Coordination between different barriers?</t>
+  </si>
+  <si>
+    <t>How does optimal timeout value varies with the deadline value. Is it D/2? If both the distributions are same</t>
+  </si>
+  <si>
+    <t>Amazon EC2 results -- First repeat simulation results, then go on running on a weak testbed to evaluate</t>
+  </si>
+  <si>
+    <t>01/21/2013</t>
+  </si>
+  <si>
+    <t>First answer Ion's question about optimal timeout value. Is it D/2?</t>
+  </si>
+  <si>
+    <t>D/2 is not so bad. -- Do Theoretical analysis.</t>
+  </si>
+  <si>
+    <t>OptimalTimeoutVsDeadline.py</t>
+  </si>
+  <si>
+    <t>Iterative computation</t>
   </si>
 </sst>
 </file>
@@ -104,8 +227,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -114,9 +257,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,15 +558,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1">
         <v>41101</v>
       </c>
@@ -411,7 +577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -419,7 +585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>40980</v>
       </c>
@@ -427,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>41011</v>
       </c>
@@ -438,12 +604,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:7">
       <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>41041</v>
       </c>
@@ -454,17 +620,252 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:7">
       <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:7">
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>41426</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>41456</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>41518</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>41548</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="D42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>